<commit_message>
Added full name to the Estados column
</commit_message>
<xml_diff>
--- a/Datos/INEGI/Mexico/pobreza_sonora_processed.xlsx
+++ b/Datos/INEGI/Mexico/pobreza_sonora_processed.xlsx
@@ -605,7 +605,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>EUM</t>
+          <t>Estados Unidos Mexicanos</t>
         </is>
       </c>
     </row>
@@ -662,7 +662,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>EUM</t>
+          <t>Estados Unidos Mexicanos</t>
         </is>
       </c>
     </row>
@@ -719,7 +719,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>EUM</t>
+          <t>Estados Unidos Mexicanos</t>
         </is>
       </c>
     </row>
@@ -776,7 +776,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>EUM</t>
+          <t>Estados Unidos Mexicanos</t>
         </is>
       </c>
     </row>
@@ -833,7 +833,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>EUM</t>
+          <t>Estados Unidos Mexicanos</t>
         </is>
       </c>
     </row>
@@ -890,7 +890,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>EUM</t>
+          <t>Estados Unidos Mexicanos</t>
         </is>
       </c>
     </row>
@@ -947,7 +947,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>EUM</t>
+          <t>Estados Unidos Mexicanos</t>
         </is>
       </c>
     </row>
@@ -1004,7 +1004,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>EUM</t>
+          <t>Estados Unidos Mexicanos</t>
         </is>
       </c>
     </row>
@@ -1061,7 +1061,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>EUM</t>
+          <t>Estados Unidos Mexicanos</t>
         </is>
       </c>
     </row>
@@ -1118,7 +1118,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>EUM</t>
+          <t>Estados Unidos Mexicanos</t>
         </is>
       </c>
     </row>
@@ -1175,7 +1175,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>EUM</t>
+          <t>Estados Unidos Mexicanos</t>
         </is>
       </c>
     </row>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>EUM</t>
+          <t>Estados Unidos Mexicanos</t>
         </is>
       </c>
     </row>
@@ -1289,7 +1289,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>EUM</t>
+          <t>Estados Unidos Mexicanos</t>
         </is>
       </c>
     </row>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>EUM</t>
+          <t>Estados Unidos Mexicanos</t>
         </is>
       </c>
     </row>
@@ -1403,7 +1403,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>EUM</t>
+          <t>Estados Unidos Mexicanos</t>
         </is>
       </c>
     </row>
@@ -1460,7 +1460,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>EUM</t>
+          <t>Estados Unidos Mexicanos</t>
         </is>
       </c>
     </row>
@@ -1623,7 +1623,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>CDMX</t>
+          <t>Ciudad de México</t>
         </is>
       </c>
     </row>
@@ -1680,7 +1680,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>CDMX</t>
+          <t>Ciudad de México</t>
         </is>
       </c>
     </row>
@@ -1737,7 +1737,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>CDMX</t>
+          <t>Ciudad de México</t>
         </is>
       </c>
     </row>
@@ -1794,7 +1794,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>CDMX</t>
+          <t>Ciudad de México</t>
         </is>
       </c>
     </row>
@@ -1851,7 +1851,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>CDMX</t>
+          <t>Ciudad de México</t>
         </is>
       </c>
     </row>
@@ -1908,7 +1908,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>CDMX</t>
+          <t>Ciudad de México</t>
         </is>
       </c>
     </row>
@@ -1965,7 +1965,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>CDMX</t>
+          <t>Ciudad de México</t>
         </is>
       </c>
     </row>
@@ -2022,7 +2022,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>CDMX</t>
+          <t>Ciudad de México</t>
         </is>
       </c>
     </row>
@@ -2079,7 +2079,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>CDMX</t>
+          <t>Ciudad de México</t>
         </is>
       </c>
     </row>
@@ -2136,7 +2136,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>CDMX</t>
+          <t>Ciudad de México</t>
         </is>
       </c>
     </row>
@@ -2193,7 +2193,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>CDMX</t>
+          <t>Ciudad de México</t>
         </is>
       </c>
     </row>
@@ -2250,7 +2250,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>CDMX</t>
+          <t>Ciudad de México</t>
         </is>
       </c>
     </row>
@@ -2307,7 +2307,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>CDMX</t>
+          <t>Ciudad de México</t>
         </is>
       </c>
     </row>
@@ -2364,7 +2364,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>CDMX</t>
+          <t>Ciudad de México</t>
         </is>
       </c>
     </row>
@@ -2421,7 +2421,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>CDMX</t>
+          <t>Ciudad de México</t>
         </is>
       </c>
     </row>
@@ -2478,7 +2478,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>CDMX</t>
+          <t>Ciudad de México</t>
         </is>
       </c>
     </row>
@@ -2641,7 +2641,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Dgo.</t>
+          <t>Durango</t>
         </is>
       </c>
     </row>
@@ -2698,7 +2698,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Dgo.</t>
+          <t>Durango</t>
         </is>
       </c>
     </row>
@@ -2755,7 +2755,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Dgo.</t>
+          <t>Durango</t>
         </is>
       </c>
     </row>
@@ -2812,7 +2812,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Dgo.</t>
+          <t>Durango</t>
         </is>
       </c>
     </row>
@@ -2869,7 +2869,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Dgo.</t>
+          <t>Durango</t>
         </is>
       </c>
     </row>
@@ -2926,7 +2926,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Dgo.</t>
+          <t>Durango</t>
         </is>
       </c>
     </row>
@@ -2983,7 +2983,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Dgo.</t>
+          <t>Durango</t>
         </is>
       </c>
     </row>
@@ -3040,7 +3040,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Dgo.</t>
+          <t>Durango</t>
         </is>
       </c>
     </row>
@@ -3097,7 +3097,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Dgo.</t>
+          <t>Durango</t>
         </is>
       </c>
     </row>
@@ -3154,7 +3154,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Dgo.</t>
+          <t>Durango</t>
         </is>
       </c>
     </row>
@@ -3211,7 +3211,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>Dgo.</t>
+          <t>Durango</t>
         </is>
       </c>
     </row>
@@ -3268,7 +3268,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Dgo.</t>
+          <t>Durango</t>
         </is>
       </c>
     </row>
@@ -3325,7 +3325,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>Dgo.</t>
+          <t>Durango</t>
         </is>
       </c>
     </row>
@@ -3382,7 +3382,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>Dgo.</t>
+          <t>Durango</t>
         </is>
       </c>
     </row>
@@ -3439,7 +3439,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>Dgo.</t>
+          <t>Durango</t>
         </is>
       </c>
     </row>
@@ -3496,7 +3496,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>Dgo.</t>
+          <t>Durango</t>
         </is>
       </c>
     </row>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Gto.</t>
+          <t>Guanajuato</t>
         </is>
       </c>
     </row>
@@ -3716,7 +3716,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Gto.</t>
+          <t>Guanajuato</t>
         </is>
       </c>
     </row>
@@ -3773,7 +3773,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Gto.</t>
+          <t>Guanajuato</t>
         </is>
       </c>
     </row>
@@ -3830,7 +3830,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Gto.</t>
+          <t>Guanajuato</t>
         </is>
       </c>
     </row>
@@ -3887,7 +3887,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Gto.</t>
+          <t>Guanajuato</t>
         </is>
       </c>
     </row>
@@ -3944,7 +3944,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Gto.</t>
+          <t>Guanajuato</t>
         </is>
       </c>
     </row>
@@ -4001,7 +4001,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Gto.</t>
+          <t>Guanajuato</t>
         </is>
       </c>
     </row>
@@ -4058,7 +4058,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Gto.</t>
+          <t>Guanajuato</t>
         </is>
       </c>
     </row>
@@ -4115,7 +4115,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Gto.</t>
+          <t>Guanajuato</t>
         </is>
       </c>
     </row>
@@ -4172,7 +4172,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Gto.</t>
+          <t>Guanajuato</t>
         </is>
       </c>
     </row>
@@ -4229,7 +4229,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>Gto.</t>
+          <t>Guanajuato</t>
         </is>
       </c>
     </row>
@@ -4286,7 +4286,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Gto.</t>
+          <t>Guanajuato</t>
         </is>
       </c>
     </row>
@@ -4343,7 +4343,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>Gto.</t>
+          <t>Guanajuato</t>
         </is>
       </c>
     </row>
@@ -4400,7 +4400,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>Gto.</t>
+          <t>Guanajuato</t>
         </is>
       </c>
     </row>
@@ -4457,7 +4457,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>Gto.</t>
+          <t>Guanajuato</t>
         </is>
       </c>
     </row>
@@ -4514,7 +4514,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>Gto.</t>
+          <t>Guanajuato</t>
         </is>
       </c>
     </row>
@@ -4677,7 +4677,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Gro.</t>
+          <t>Guerrero</t>
         </is>
       </c>
     </row>
@@ -4734,7 +4734,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Gro.</t>
+          <t>Guerrero</t>
         </is>
       </c>
     </row>
@@ -4791,7 +4791,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Gro.</t>
+          <t>Guerrero</t>
         </is>
       </c>
     </row>
@@ -4848,7 +4848,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Gro.</t>
+          <t>Guerrero</t>
         </is>
       </c>
     </row>
@@ -4905,7 +4905,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Gro.</t>
+          <t>Guerrero</t>
         </is>
       </c>
     </row>
@@ -4962,7 +4962,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Gro.</t>
+          <t>Guerrero</t>
         </is>
       </c>
     </row>
@@ -5019,7 +5019,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Gro.</t>
+          <t>Guerrero</t>
         </is>
       </c>
     </row>
@@ -5076,7 +5076,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Gro.</t>
+          <t>Guerrero</t>
         </is>
       </c>
     </row>
@@ -5133,7 +5133,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Gro.</t>
+          <t>Guerrero</t>
         </is>
       </c>
     </row>
@@ -5190,7 +5190,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Gro.</t>
+          <t>Guerrero</t>
         </is>
       </c>
     </row>
@@ -5247,7 +5247,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>Gro.</t>
+          <t>Guerrero</t>
         </is>
       </c>
     </row>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Gro.</t>
+          <t>Guerrero</t>
         </is>
       </c>
     </row>
@@ -5361,7 +5361,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>Gro.</t>
+          <t>Guerrero</t>
         </is>
       </c>
     </row>
@@ -5418,7 +5418,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>Gro.</t>
+          <t>Guerrero</t>
         </is>
       </c>
     </row>
@@ -5475,7 +5475,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>Gro.</t>
+          <t>Guerrero</t>
         </is>
       </c>
     </row>
@@ -5532,7 +5532,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>Gro.</t>
+          <t>Guerrero</t>
         </is>
       </c>
     </row>
@@ -5695,7 +5695,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Hgo.</t>
+          <t>Hidalgo</t>
         </is>
       </c>
     </row>
@@ -5752,7 +5752,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Hgo.</t>
+          <t>Hidalgo</t>
         </is>
       </c>
     </row>
@@ -5809,7 +5809,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Hgo.</t>
+          <t>Hidalgo</t>
         </is>
       </c>
     </row>
@@ -5866,7 +5866,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Hgo.</t>
+          <t>Hidalgo</t>
         </is>
       </c>
     </row>
@@ -5923,7 +5923,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Hgo.</t>
+          <t>Hidalgo</t>
         </is>
       </c>
     </row>
@@ -5980,7 +5980,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Hgo.</t>
+          <t>Hidalgo</t>
         </is>
       </c>
     </row>
@@ -6037,7 +6037,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Hgo.</t>
+          <t>Hidalgo</t>
         </is>
       </c>
     </row>
@@ -6094,7 +6094,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Hgo.</t>
+          <t>Hidalgo</t>
         </is>
       </c>
     </row>
@@ -6151,7 +6151,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Hgo.</t>
+          <t>Hidalgo</t>
         </is>
       </c>
     </row>
@@ -6208,7 +6208,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Hgo.</t>
+          <t>Hidalgo</t>
         </is>
       </c>
     </row>
@@ -6265,7 +6265,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>Hgo.</t>
+          <t>Hidalgo</t>
         </is>
       </c>
     </row>
@@ -6322,7 +6322,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Hgo.</t>
+          <t>Hidalgo</t>
         </is>
       </c>
     </row>
@@ -6379,7 +6379,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>Hgo.</t>
+          <t>Hidalgo</t>
         </is>
       </c>
     </row>
@@ -6436,7 +6436,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>Hgo.</t>
+          <t>Hidalgo</t>
         </is>
       </c>
     </row>
@@ -6493,7 +6493,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>Hgo.</t>
+          <t>Hidalgo</t>
         </is>
       </c>
     </row>
@@ -6550,7 +6550,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>Hgo.</t>
+          <t>Hidalgo</t>
         </is>
       </c>
     </row>
@@ -6713,7 +6713,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Jal.</t>
+          <t>Jalisco</t>
         </is>
       </c>
     </row>
@@ -6770,7 +6770,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Jal.</t>
+          <t>Jalisco</t>
         </is>
       </c>
     </row>
@@ -6827,7 +6827,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Jal.</t>
+          <t>Jalisco</t>
         </is>
       </c>
     </row>
@@ -6884,7 +6884,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Jal.</t>
+          <t>Jalisco</t>
         </is>
       </c>
     </row>
@@ -6941,7 +6941,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Jal.</t>
+          <t>Jalisco</t>
         </is>
       </c>
     </row>
@@ -6998,7 +6998,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Jal.</t>
+          <t>Jalisco</t>
         </is>
       </c>
     </row>
@@ -7055,7 +7055,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Jal.</t>
+          <t>Jalisco</t>
         </is>
       </c>
     </row>
@@ -7112,7 +7112,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Jal.</t>
+          <t>Jalisco</t>
         </is>
       </c>
     </row>
@@ -7169,7 +7169,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Jal.</t>
+          <t>Jalisco</t>
         </is>
       </c>
     </row>
@@ -7226,7 +7226,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Jal.</t>
+          <t>Jalisco</t>
         </is>
       </c>
     </row>
@@ -7283,7 +7283,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>Jal.</t>
+          <t>Jalisco</t>
         </is>
       </c>
     </row>
@@ -7340,7 +7340,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Jal.</t>
+          <t>Jalisco</t>
         </is>
       </c>
     </row>
@@ -7397,7 +7397,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>Jal.</t>
+          <t>Jalisco</t>
         </is>
       </c>
     </row>
@@ -7454,7 +7454,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>Jal.</t>
+          <t>Jalisco</t>
         </is>
       </c>
     </row>
@@ -7511,7 +7511,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>Jal.</t>
+          <t>Jalisco</t>
         </is>
       </c>
     </row>
@@ -7568,7 +7568,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>Jal.</t>
+          <t>Jalisco</t>
         </is>
       </c>
     </row>
@@ -7731,7 +7731,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Mex.</t>
+          <t>Estado de México</t>
         </is>
       </c>
     </row>
@@ -7788,7 +7788,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Mex.</t>
+          <t>Estado de México</t>
         </is>
       </c>
     </row>
@@ -7845,7 +7845,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Mex.</t>
+          <t>Estado de México</t>
         </is>
       </c>
     </row>
@@ -7902,7 +7902,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Mex.</t>
+          <t>Estado de México</t>
         </is>
       </c>
     </row>
@@ -7959,7 +7959,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Mex.</t>
+          <t>Estado de México</t>
         </is>
       </c>
     </row>
@@ -8016,7 +8016,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Mex.</t>
+          <t>Estado de México</t>
         </is>
       </c>
     </row>
@@ -8073,7 +8073,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Mex.</t>
+          <t>Estado de México</t>
         </is>
       </c>
     </row>
@@ -8130,7 +8130,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Mex.</t>
+          <t>Estado de México</t>
         </is>
       </c>
     </row>
@@ -8187,7 +8187,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Mex.</t>
+          <t>Estado de México</t>
         </is>
       </c>
     </row>
@@ -8244,7 +8244,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Mex.</t>
+          <t>Estado de México</t>
         </is>
       </c>
     </row>
@@ -8301,7 +8301,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>Mex.</t>
+          <t>Estado de México</t>
         </is>
       </c>
     </row>
@@ -8358,7 +8358,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Mex.</t>
+          <t>Estado de México</t>
         </is>
       </c>
     </row>
@@ -8415,7 +8415,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>Mex.</t>
+          <t>Estado de México</t>
         </is>
       </c>
     </row>
@@ -8472,7 +8472,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>Mex.</t>
+          <t>Estado de México</t>
         </is>
       </c>
     </row>
@@ -8529,7 +8529,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>Mex.</t>
+          <t>Estado de México</t>
         </is>
       </c>
     </row>
@@ -8586,7 +8586,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>Mex.</t>
+          <t>Estado de México</t>
         </is>
       </c>
     </row>
@@ -8749,7 +8749,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Mich.</t>
+          <t>Michoacán</t>
         </is>
       </c>
     </row>
@@ -8806,7 +8806,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Mich.</t>
+          <t>Michoacán</t>
         </is>
       </c>
     </row>
@@ -8863,7 +8863,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Mich.</t>
+          <t>Michoacán</t>
         </is>
       </c>
     </row>
@@ -8920,7 +8920,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Mich.</t>
+          <t>Michoacán</t>
         </is>
       </c>
     </row>
@@ -8977,7 +8977,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Mich.</t>
+          <t>Michoacán</t>
         </is>
       </c>
     </row>
@@ -9034,7 +9034,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Mich.</t>
+          <t>Michoacán</t>
         </is>
       </c>
     </row>
@@ -9091,7 +9091,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Mich.</t>
+          <t>Michoacán</t>
         </is>
       </c>
     </row>
@@ -9148,7 +9148,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Mich.</t>
+          <t>Michoacán</t>
         </is>
       </c>
     </row>
@@ -9205,7 +9205,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Mich.</t>
+          <t>Michoacán</t>
         </is>
       </c>
     </row>
@@ -9262,7 +9262,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Mich.</t>
+          <t>Michoacán</t>
         </is>
       </c>
     </row>
@@ -9319,7 +9319,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>Mich.</t>
+          <t>Michoacán</t>
         </is>
       </c>
     </row>
@@ -9376,7 +9376,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Mich.</t>
+          <t>Michoacán</t>
         </is>
       </c>
     </row>
@@ -9433,7 +9433,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>Mich.</t>
+          <t>Michoacán</t>
         </is>
       </c>
     </row>
@@ -9490,7 +9490,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>Mich.</t>
+          <t>Michoacán</t>
         </is>
       </c>
     </row>
@@ -9547,7 +9547,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>Mich.</t>
+          <t>Michoacán</t>
         </is>
       </c>
     </row>
@@ -9604,7 +9604,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>Mich.</t>
+          <t>Michoacán</t>
         </is>
       </c>
     </row>
@@ -9767,7 +9767,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Mor.</t>
+          <t>Morelos</t>
         </is>
       </c>
     </row>
@@ -9824,7 +9824,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Mor.</t>
+          <t>Morelos</t>
         </is>
       </c>
     </row>
@@ -9881,7 +9881,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Mor.</t>
+          <t>Morelos</t>
         </is>
       </c>
     </row>
@@ -9938,7 +9938,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Mor.</t>
+          <t>Morelos</t>
         </is>
       </c>
     </row>
@@ -9995,7 +9995,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Mor.</t>
+          <t>Morelos</t>
         </is>
       </c>
     </row>
@@ -10052,7 +10052,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Mor.</t>
+          <t>Morelos</t>
         </is>
       </c>
     </row>
@@ -10109,7 +10109,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Mor.</t>
+          <t>Morelos</t>
         </is>
       </c>
     </row>
@@ -10166,7 +10166,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Mor.</t>
+          <t>Morelos</t>
         </is>
       </c>
     </row>
@@ -10223,7 +10223,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Mor.</t>
+          <t>Morelos</t>
         </is>
       </c>
     </row>
@@ -10280,7 +10280,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Mor.</t>
+          <t>Morelos</t>
         </is>
       </c>
     </row>
@@ -10337,7 +10337,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>Mor.</t>
+          <t>Morelos</t>
         </is>
       </c>
     </row>
@@ -10394,7 +10394,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Mor.</t>
+          <t>Morelos</t>
         </is>
       </c>
     </row>
@@ -10451,7 +10451,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>Mor.</t>
+          <t>Morelos</t>
         </is>
       </c>
     </row>
@@ -10508,7 +10508,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>Mor.</t>
+          <t>Morelos</t>
         </is>
       </c>
     </row>
@@ -10565,7 +10565,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>Mor.</t>
+          <t>Morelos</t>
         </is>
       </c>
     </row>
@@ -10622,7 +10622,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>Mor.</t>
+          <t>Morelos</t>
         </is>
       </c>
     </row>
@@ -10785,7 +10785,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Nay.</t>
+          <t>Nayarit</t>
         </is>
       </c>
     </row>
@@ -10842,7 +10842,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Nay.</t>
+          <t>Nayarit</t>
         </is>
       </c>
     </row>
@@ -10899,7 +10899,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Nay.</t>
+          <t>Nayarit</t>
         </is>
       </c>
     </row>
@@ -10956,7 +10956,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Nay.</t>
+          <t>Nayarit</t>
         </is>
       </c>
     </row>
@@ -11013,7 +11013,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Nay.</t>
+          <t>Nayarit</t>
         </is>
       </c>
     </row>
@@ -11070,7 +11070,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Nay.</t>
+          <t>Nayarit</t>
         </is>
       </c>
     </row>
@@ -11127,7 +11127,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Nay.</t>
+          <t>Nayarit</t>
         </is>
       </c>
     </row>
@@ -11184,7 +11184,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Nay.</t>
+          <t>Nayarit</t>
         </is>
       </c>
     </row>
@@ -11241,7 +11241,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Nay.</t>
+          <t>Nayarit</t>
         </is>
       </c>
     </row>
@@ -11298,7 +11298,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Nay.</t>
+          <t>Nayarit</t>
         </is>
       </c>
     </row>
@@ -11355,7 +11355,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>Nay.</t>
+          <t>Nayarit</t>
         </is>
       </c>
     </row>
@@ -11412,7 +11412,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Nay.</t>
+          <t>Nayarit</t>
         </is>
       </c>
     </row>
@@ -11469,7 +11469,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>Nay.</t>
+          <t>Nayarit</t>
         </is>
       </c>
     </row>
@@ -11526,7 +11526,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>Nay.</t>
+          <t>Nayarit</t>
         </is>
       </c>
     </row>
@@ -11583,7 +11583,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>Nay.</t>
+          <t>Nayarit</t>
         </is>
       </c>
     </row>
@@ -11640,7 +11640,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>Nay.</t>
+          <t>Nayarit</t>
         </is>
       </c>
     </row>
@@ -11803,7 +11803,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Ags.</t>
+          <t>Aguascalientes</t>
         </is>
       </c>
     </row>
@@ -11860,7 +11860,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Ags.</t>
+          <t>Aguascalientes</t>
         </is>
       </c>
     </row>
@@ -11917,7 +11917,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Ags.</t>
+          <t>Aguascalientes</t>
         </is>
       </c>
     </row>
@@ -11974,7 +11974,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Ags.</t>
+          <t>Aguascalientes</t>
         </is>
       </c>
     </row>
@@ -12031,7 +12031,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Ags.</t>
+          <t>Aguascalientes</t>
         </is>
       </c>
     </row>
@@ -12088,7 +12088,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Ags.</t>
+          <t>Aguascalientes</t>
         </is>
       </c>
     </row>
@@ -12145,7 +12145,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Ags.</t>
+          <t>Aguascalientes</t>
         </is>
       </c>
     </row>
@@ -12202,7 +12202,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Ags.</t>
+          <t>Aguascalientes</t>
         </is>
       </c>
     </row>
@@ -12259,7 +12259,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Ags.</t>
+          <t>Aguascalientes</t>
         </is>
       </c>
     </row>
@@ -12316,7 +12316,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Ags.</t>
+          <t>Aguascalientes</t>
         </is>
       </c>
     </row>
@@ -12373,7 +12373,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>Ags.</t>
+          <t>Aguascalientes</t>
         </is>
       </c>
     </row>
@@ -12430,7 +12430,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Ags.</t>
+          <t>Aguascalientes</t>
         </is>
       </c>
     </row>
@@ -12487,7 +12487,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>Ags.</t>
+          <t>Aguascalientes</t>
         </is>
       </c>
     </row>
@@ -12544,7 +12544,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>Ags.</t>
+          <t>Aguascalientes</t>
         </is>
       </c>
     </row>
@@ -12601,7 +12601,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>Ags.</t>
+          <t>Aguascalientes</t>
         </is>
       </c>
     </row>
@@ -12658,7 +12658,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>Ags.</t>
+          <t>Aguascalientes</t>
         </is>
       </c>
     </row>
@@ -12821,7 +12821,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>NL</t>
+          <t>Nuevo León</t>
         </is>
       </c>
     </row>
@@ -12878,7 +12878,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>NL</t>
+          <t>Nuevo León</t>
         </is>
       </c>
     </row>
@@ -12935,7 +12935,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>NL</t>
+          <t>Nuevo León</t>
         </is>
       </c>
     </row>
@@ -12992,7 +12992,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>NL</t>
+          <t>Nuevo León</t>
         </is>
       </c>
     </row>
@@ -13049,7 +13049,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>NL</t>
+          <t>Nuevo León</t>
         </is>
       </c>
     </row>
@@ -13106,7 +13106,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>NL</t>
+          <t>Nuevo León</t>
         </is>
       </c>
     </row>
@@ -13163,7 +13163,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>NL</t>
+          <t>Nuevo León</t>
         </is>
       </c>
     </row>
@@ -13220,7 +13220,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>NL</t>
+          <t>Nuevo León</t>
         </is>
       </c>
     </row>
@@ -13277,7 +13277,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>NL</t>
+          <t>Nuevo León</t>
         </is>
       </c>
     </row>
@@ -13334,7 +13334,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>NL</t>
+          <t>Nuevo León</t>
         </is>
       </c>
     </row>
@@ -13391,7 +13391,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>NL</t>
+          <t>Nuevo León</t>
         </is>
       </c>
     </row>
@@ -13448,7 +13448,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>NL</t>
+          <t>Nuevo León</t>
         </is>
       </c>
     </row>
@@ -13505,7 +13505,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>NL</t>
+          <t>Nuevo León</t>
         </is>
       </c>
     </row>
@@ -13562,7 +13562,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>NL</t>
+          <t>Nuevo León</t>
         </is>
       </c>
     </row>
@@ -13619,7 +13619,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>NL</t>
+          <t>Nuevo León</t>
         </is>
       </c>
     </row>
@@ -13676,7 +13676,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>NL</t>
+          <t>Nuevo León</t>
         </is>
       </c>
     </row>
@@ -13839,7 +13839,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Oax.</t>
+          <t>Oaxaca</t>
         </is>
       </c>
     </row>
@@ -13896,7 +13896,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Oax.</t>
+          <t>Oaxaca</t>
         </is>
       </c>
     </row>
@@ -13953,7 +13953,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Oax.</t>
+          <t>Oaxaca</t>
         </is>
       </c>
     </row>
@@ -14010,7 +14010,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Oax.</t>
+          <t>Oaxaca</t>
         </is>
       </c>
     </row>
@@ -14067,7 +14067,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Oax.</t>
+          <t>Oaxaca</t>
         </is>
       </c>
     </row>
@@ -14124,7 +14124,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Oax.</t>
+          <t>Oaxaca</t>
         </is>
       </c>
     </row>
@@ -14181,7 +14181,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Oax.</t>
+          <t>Oaxaca</t>
         </is>
       </c>
     </row>
@@ -14238,7 +14238,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Oax.</t>
+          <t>Oaxaca</t>
         </is>
       </c>
     </row>
@@ -14295,7 +14295,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Oax.</t>
+          <t>Oaxaca</t>
         </is>
       </c>
     </row>
@@ -14352,7 +14352,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Oax.</t>
+          <t>Oaxaca</t>
         </is>
       </c>
     </row>
@@ -14409,7 +14409,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>Oax.</t>
+          <t>Oaxaca</t>
         </is>
       </c>
     </row>
@@ -14466,7 +14466,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Oax.</t>
+          <t>Oaxaca</t>
         </is>
       </c>
     </row>
@@ -14523,7 +14523,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>Oax.</t>
+          <t>Oaxaca</t>
         </is>
       </c>
     </row>
@@ -14580,7 +14580,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>Oax.</t>
+          <t>Oaxaca</t>
         </is>
       </c>
     </row>
@@ -14637,7 +14637,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>Oax.</t>
+          <t>Oaxaca</t>
         </is>
       </c>
     </row>
@@ -14694,7 +14694,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>Oax.</t>
+          <t>Oaxaca</t>
         </is>
       </c>
     </row>
@@ -14857,7 +14857,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Pue.</t>
+          <t>Puebla</t>
         </is>
       </c>
     </row>
@@ -14914,7 +14914,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Pue.</t>
+          <t>Puebla</t>
         </is>
       </c>
     </row>
@@ -14971,7 +14971,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Pue.</t>
+          <t>Puebla</t>
         </is>
       </c>
     </row>
@@ -15028,7 +15028,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Pue.</t>
+          <t>Puebla</t>
         </is>
       </c>
     </row>
@@ -15085,7 +15085,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Pue.</t>
+          <t>Puebla</t>
         </is>
       </c>
     </row>
@@ -15142,7 +15142,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Pue.</t>
+          <t>Puebla</t>
         </is>
       </c>
     </row>
@@ -15199,7 +15199,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Pue.</t>
+          <t>Puebla</t>
         </is>
       </c>
     </row>
@@ -15256,7 +15256,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Pue.</t>
+          <t>Puebla</t>
         </is>
       </c>
     </row>
@@ -15313,7 +15313,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Pue.</t>
+          <t>Puebla</t>
         </is>
       </c>
     </row>
@@ -15370,7 +15370,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Pue.</t>
+          <t>Puebla</t>
         </is>
       </c>
     </row>
@@ -15427,7 +15427,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>Pue.</t>
+          <t>Puebla</t>
         </is>
       </c>
     </row>
@@ -15484,7 +15484,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Pue.</t>
+          <t>Puebla</t>
         </is>
       </c>
     </row>
@@ -15541,7 +15541,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>Pue.</t>
+          <t>Puebla</t>
         </is>
       </c>
     </row>
@@ -15598,7 +15598,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>Pue.</t>
+          <t>Puebla</t>
         </is>
       </c>
     </row>
@@ -15655,7 +15655,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>Pue.</t>
+          <t>Puebla</t>
         </is>
       </c>
     </row>
@@ -15712,7 +15712,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>Pue.</t>
+          <t>Puebla</t>
         </is>
       </c>
     </row>
@@ -15875,7 +15875,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Qro.</t>
+          <t>Querétaro</t>
         </is>
       </c>
     </row>
@@ -15932,7 +15932,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Qro.</t>
+          <t>Querétaro</t>
         </is>
       </c>
     </row>
@@ -15989,7 +15989,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Qro.</t>
+          <t>Querétaro</t>
         </is>
       </c>
     </row>
@@ -16046,7 +16046,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Qro.</t>
+          <t>Querétaro</t>
         </is>
       </c>
     </row>
@@ -16103,7 +16103,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Qro.</t>
+          <t>Querétaro</t>
         </is>
       </c>
     </row>
@@ -16160,7 +16160,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Qro.</t>
+          <t>Querétaro</t>
         </is>
       </c>
     </row>
@@ -16217,7 +16217,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Qro.</t>
+          <t>Querétaro</t>
         </is>
       </c>
     </row>
@@ -16274,7 +16274,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Qro.</t>
+          <t>Querétaro</t>
         </is>
       </c>
     </row>
@@ -16331,7 +16331,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Qro.</t>
+          <t>Querétaro</t>
         </is>
       </c>
     </row>
@@ -16388,7 +16388,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Qro.</t>
+          <t>Querétaro</t>
         </is>
       </c>
     </row>
@@ -16445,7 +16445,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>Qro.</t>
+          <t>Querétaro</t>
         </is>
       </c>
     </row>
@@ -16502,7 +16502,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Qro.</t>
+          <t>Querétaro</t>
         </is>
       </c>
     </row>
@@ -16559,7 +16559,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>Qro.</t>
+          <t>Querétaro</t>
         </is>
       </c>
     </row>
@@ -16616,7 +16616,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>Qro.</t>
+          <t>Querétaro</t>
         </is>
       </c>
     </row>
@@ -16673,7 +16673,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>Qro.</t>
+          <t>Querétaro</t>
         </is>
       </c>
     </row>
@@ -16730,7 +16730,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>Qro.</t>
+          <t>Querétaro</t>
         </is>
       </c>
     </row>
@@ -16893,7 +16893,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Q. Roo</t>
+          <t>Quintana Roo</t>
         </is>
       </c>
     </row>
@@ -16950,7 +16950,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Q. Roo</t>
+          <t>Quintana Roo</t>
         </is>
       </c>
     </row>
@@ -17007,7 +17007,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Q. Roo</t>
+          <t>Quintana Roo</t>
         </is>
       </c>
     </row>
@@ -17064,7 +17064,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Q. Roo</t>
+          <t>Quintana Roo</t>
         </is>
       </c>
     </row>
@@ -17121,7 +17121,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Q. Roo</t>
+          <t>Quintana Roo</t>
         </is>
       </c>
     </row>
@@ -17178,7 +17178,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Q. Roo</t>
+          <t>Quintana Roo</t>
         </is>
       </c>
     </row>
@@ -17235,7 +17235,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Q. Roo</t>
+          <t>Quintana Roo</t>
         </is>
       </c>
     </row>
@@ -17292,7 +17292,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Q. Roo</t>
+          <t>Quintana Roo</t>
         </is>
       </c>
     </row>
@@ -17349,7 +17349,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Q. Roo</t>
+          <t>Quintana Roo</t>
         </is>
       </c>
     </row>
@@ -17406,7 +17406,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Q. Roo</t>
+          <t>Quintana Roo</t>
         </is>
       </c>
     </row>
@@ -17463,7 +17463,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>Q. Roo</t>
+          <t>Quintana Roo</t>
         </is>
       </c>
     </row>
@@ -17520,7 +17520,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Q. Roo</t>
+          <t>Quintana Roo</t>
         </is>
       </c>
     </row>
@@ -17577,7 +17577,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>Q. Roo</t>
+          <t>Quintana Roo</t>
         </is>
       </c>
     </row>
@@ -17634,7 +17634,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>Q. Roo</t>
+          <t>Quintana Roo</t>
         </is>
       </c>
     </row>
@@ -17691,7 +17691,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>Q. Roo</t>
+          <t>Quintana Roo</t>
         </is>
       </c>
     </row>
@@ -17748,7 +17748,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>Q. Roo</t>
+          <t>Quintana Roo</t>
         </is>
       </c>
     </row>
@@ -17911,7 +17911,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>SLP</t>
+          <t>San Luis Potosí</t>
         </is>
       </c>
     </row>
@@ -17968,7 +17968,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>SLP</t>
+          <t>San Luis Potosí</t>
         </is>
       </c>
     </row>
@@ -18025,7 +18025,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>SLP</t>
+          <t>San Luis Potosí</t>
         </is>
       </c>
     </row>
@@ -18082,7 +18082,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>SLP</t>
+          <t>San Luis Potosí</t>
         </is>
       </c>
     </row>
@@ -18139,7 +18139,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>SLP</t>
+          <t>San Luis Potosí</t>
         </is>
       </c>
     </row>
@@ -18196,7 +18196,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>SLP</t>
+          <t>San Luis Potosí</t>
         </is>
       </c>
     </row>
@@ -18253,7 +18253,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>SLP</t>
+          <t>San Luis Potosí</t>
         </is>
       </c>
     </row>
@@ -18310,7 +18310,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>SLP</t>
+          <t>San Luis Potosí</t>
         </is>
       </c>
     </row>
@@ -18367,7 +18367,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>SLP</t>
+          <t>San Luis Potosí</t>
         </is>
       </c>
     </row>
@@ -18424,7 +18424,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>SLP</t>
+          <t>San Luis Potosí</t>
         </is>
       </c>
     </row>
@@ -18481,7 +18481,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>SLP</t>
+          <t>San Luis Potosí</t>
         </is>
       </c>
     </row>
@@ -18538,7 +18538,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>SLP</t>
+          <t>San Luis Potosí</t>
         </is>
       </c>
     </row>
@@ -18595,7 +18595,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>SLP</t>
+          <t>San Luis Potosí</t>
         </is>
       </c>
     </row>
@@ -18652,7 +18652,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>SLP</t>
+          <t>San Luis Potosí</t>
         </is>
       </c>
     </row>
@@ -18709,7 +18709,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>SLP</t>
+          <t>San Luis Potosí</t>
         </is>
       </c>
     </row>
@@ -18766,7 +18766,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>SLP</t>
+          <t>San Luis Potosí</t>
         </is>
       </c>
     </row>
@@ -18929,7 +18929,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Sin.</t>
+          <t>Sinaloa</t>
         </is>
       </c>
     </row>
@@ -18986,7 +18986,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Sin.</t>
+          <t>Sinaloa</t>
         </is>
       </c>
     </row>
@@ -19043,7 +19043,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Sin.</t>
+          <t>Sinaloa</t>
         </is>
       </c>
     </row>
@@ -19100,7 +19100,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Sin.</t>
+          <t>Sinaloa</t>
         </is>
       </c>
     </row>
@@ -19157,7 +19157,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Sin.</t>
+          <t>Sinaloa</t>
         </is>
       </c>
     </row>
@@ -19214,7 +19214,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Sin.</t>
+          <t>Sinaloa</t>
         </is>
       </c>
     </row>
@@ -19271,7 +19271,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Sin.</t>
+          <t>Sinaloa</t>
         </is>
       </c>
     </row>
@@ -19328,7 +19328,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Sin.</t>
+          <t>Sinaloa</t>
         </is>
       </c>
     </row>
@@ -19385,7 +19385,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Sin.</t>
+          <t>Sinaloa</t>
         </is>
       </c>
     </row>
@@ -19442,7 +19442,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Sin.</t>
+          <t>Sinaloa</t>
         </is>
       </c>
     </row>
@@ -19499,7 +19499,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>Sin.</t>
+          <t>Sinaloa</t>
         </is>
       </c>
     </row>
@@ -19556,7 +19556,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Sin.</t>
+          <t>Sinaloa</t>
         </is>
       </c>
     </row>
@@ -19613,7 +19613,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>Sin.</t>
+          <t>Sinaloa</t>
         </is>
       </c>
     </row>
@@ -19670,7 +19670,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>Sin.</t>
+          <t>Sinaloa</t>
         </is>
       </c>
     </row>
@@ -19727,7 +19727,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>Sin.</t>
+          <t>Sinaloa</t>
         </is>
       </c>
     </row>
@@ -19784,7 +19784,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>Sin.</t>
+          <t>Sinaloa</t>
         </is>
       </c>
     </row>
@@ -19947,7 +19947,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Son.</t>
+          <t>Sonora</t>
         </is>
       </c>
     </row>
@@ -20004,7 +20004,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Son.</t>
+          <t>Sonora</t>
         </is>
       </c>
     </row>
@@ -20061,7 +20061,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Son.</t>
+          <t>Sonora</t>
         </is>
       </c>
     </row>
@@ -20118,7 +20118,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Son.</t>
+          <t>Sonora</t>
         </is>
       </c>
     </row>
@@ -20175,7 +20175,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Son.</t>
+          <t>Sonora</t>
         </is>
       </c>
     </row>
@@ -20232,7 +20232,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Son.</t>
+          <t>Sonora</t>
         </is>
       </c>
     </row>
@@ -20289,7 +20289,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Son.</t>
+          <t>Sonora</t>
         </is>
       </c>
     </row>
@@ -20346,7 +20346,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Son.</t>
+          <t>Sonora</t>
         </is>
       </c>
     </row>
@@ -20403,7 +20403,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Son.</t>
+          <t>Sonora</t>
         </is>
       </c>
     </row>
@@ -20460,7 +20460,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Son.</t>
+          <t>Sonora</t>
         </is>
       </c>
     </row>
@@ -20517,7 +20517,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>Son.</t>
+          <t>Sonora</t>
         </is>
       </c>
     </row>
@@ -20574,7 +20574,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Son.</t>
+          <t>Sonora</t>
         </is>
       </c>
     </row>
@@ -20631,7 +20631,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>Son.</t>
+          <t>Sonora</t>
         </is>
       </c>
     </row>
@@ -20688,7 +20688,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>Son.</t>
+          <t>Sonora</t>
         </is>
       </c>
     </row>
@@ -20745,7 +20745,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>Son.</t>
+          <t>Sonora</t>
         </is>
       </c>
     </row>
@@ -20802,7 +20802,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>Son.</t>
+          <t>Sonora</t>
         </is>
       </c>
     </row>
@@ -20965,7 +20965,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Tab.</t>
+          <t>Tabasco</t>
         </is>
       </c>
     </row>
@@ -21022,7 +21022,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Tab.</t>
+          <t>Tabasco</t>
         </is>
       </c>
     </row>
@@ -21079,7 +21079,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Tab.</t>
+          <t>Tabasco</t>
         </is>
       </c>
     </row>
@@ -21136,7 +21136,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Tab.</t>
+          <t>Tabasco</t>
         </is>
       </c>
     </row>
@@ -21193,7 +21193,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Tab.</t>
+          <t>Tabasco</t>
         </is>
       </c>
     </row>
@@ -21250,7 +21250,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Tab.</t>
+          <t>Tabasco</t>
         </is>
       </c>
     </row>
@@ -21307,7 +21307,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Tab.</t>
+          <t>Tabasco</t>
         </is>
       </c>
     </row>
@@ -21364,7 +21364,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Tab.</t>
+          <t>Tabasco</t>
         </is>
       </c>
     </row>
@@ -21421,7 +21421,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Tab.</t>
+          <t>Tabasco</t>
         </is>
       </c>
     </row>
@@ -21478,7 +21478,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Tab.</t>
+          <t>Tabasco</t>
         </is>
       </c>
     </row>
@@ -21535,7 +21535,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>Tab.</t>
+          <t>Tabasco</t>
         </is>
       </c>
     </row>
@@ -21592,7 +21592,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Tab.</t>
+          <t>Tabasco</t>
         </is>
       </c>
     </row>
@@ -21649,7 +21649,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>Tab.</t>
+          <t>Tabasco</t>
         </is>
       </c>
     </row>
@@ -21706,7 +21706,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>Tab.</t>
+          <t>Tabasco</t>
         </is>
       </c>
     </row>
@@ -21763,7 +21763,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>Tab.</t>
+          <t>Tabasco</t>
         </is>
       </c>
     </row>
@@ -21820,7 +21820,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>Tab.</t>
+          <t>Tabasco</t>
         </is>
       </c>
     </row>
@@ -21983,7 +21983,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Tamps.</t>
+          <t>Tamaulipas</t>
         </is>
       </c>
     </row>
@@ -22040,7 +22040,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Tamps.</t>
+          <t>Tamaulipas</t>
         </is>
       </c>
     </row>
@@ -22097,7 +22097,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Tamps.</t>
+          <t>Tamaulipas</t>
         </is>
       </c>
     </row>
@@ -22154,7 +22154,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Tamps.</t>
+          <t>Tamaulipas</t>
         </is>
       </c>
     </row>
@@ -22211,7 +22211,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Tamps.</t>
+          <t>Tamaulipas</t>
         </is>
       </c>
     </row>
@@ -22268,7 +22268,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Tamps.</t>
+          <t>Tamaulipas</t>
         </is>
       </c>
     </row>
@@ -22325,7 +22325,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Tamps.</t>
+          <t>Tamaulipas</t>
         </is>
       </c>
     </row>
@@ -22382,7 +22382,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Tamps.</t>
+          <t>Tamaulipas</t>
         </is>
       </c>
     </row>
@@ -22439,7 +22439,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Tamps.</t>
+          <t>Tamaulipas</t>
         </is>
       </c>
     </row>
@@ -22496,7 +22496,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Tamps.</t>
+          <t>Tamaulipas</t>
         </is>
       </c>
     </row>
@@ -22553,7 +22553,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>Tamps.</t>
+          <t>Tamaulipas</t>
         </is>
       </c>
     </row>
@@ -22610,7 +22610,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Tamps.</t>
+          <t>Tamaulipas</t>
         </is>
       </c>
     </row>
@@ -22667,7 +22667,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>Tamps.</t>
+          <t>Tamaulipas</t>
         </is>
       </c>
     </row>
@@ -22724,7 +22724,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>Tamps.</t>
+          <t>Tamaulipas</t>
         </is>
       </c>
     </row>
@@ -22781,7 +22781,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>Tamps.</t>
+          <t>Tamaulipas</t>
         </is>
       </c>
     </row>
@@ -22838,7 +22838,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>Tamps.</t>
+          <t>Tamaulipas</t>
         </is>
       </c>
     </row>
@@ -23001,7 +23001,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>BC</t>
+          <t>Baja California</t>
         </is>
       </c>
     </row>
@@ -23058,7 +23058,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>BC</t>
+          <t>Baja California</t>
         </is>
       </c>
     </row>
@@ -23115,7 +23115,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>BC</t>
+          <t>Baja California</t>
         </is>
       </c>
     </row>
@@ -23172,7 +23172,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>BC</t>
+          <t>Baja California</t>
         </is>
       </c>
     </row>
@@ -23229,7 +23229,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>BC</t>
+          <t>Baja California</t>
         </is>
       </c>
     </row>
@@ -23286,7 +23286,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>BC</t>
+          <t>Baja California</t>
         </is>
       </c>
     </row>
@@ -23343,7 +23343,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>BC</t>
+          <t>Baja California</t>
         </is>
       </c>
     </row>
@@ -23400,7 +23400,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>BC</t>
+          <t>Baja California</t>
         </is>
       </c>
     </row>
@@ -23457,7 +23457,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>BC</t>
+          <t>Baja California</t>
         </is>
       </c>
     </row>
@@ -23514,7 +23514,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>BC</t>
+          <t>Baja California</t>
         </is>
       </c>
     </row>
@@ -23571,7 +23571,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>BC</t>
+          <t>Baja California</t>
         </is>
       </c>
     </row>
@@ -23628,7 +23628,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>BC</t>
+          <t>Baja California</t>
         </is>
       </c>
     </row>
@@ -23685,7 +23685,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>BC</t>
+          <t>Baja California</t>
         </is>
       </c>
     </row>
@@ -23742,7 +23742,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>BC</t>
+          <t>Baja California</t>
         </is>
       </c>
     </row>
@@ -23799,7 +23799,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>BC</t>
+          <t>Baja California</t>
         </is>
       </c>
     </row>
@@ -23856,7 +23856,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>BC</t>
+          <t>Baja California</t>
         </is>
       </c>
     </row>
@@ -24019,7 +24019,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Tlax.</t>
+          <t>Tlaxcala</t>
         </is>
       </c>
     </row>
@@ -24076,7 +24076,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Tlax.</t>
+          <t>Tlaxcala</t>
         </is>
       </c>
     </row>
@@ -24133,7 +24133,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Tlax.</t>
+          <t>Tlaxcala</t>
         </is>
       </c>
     </row>
@@ -24190,7 +24190,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Tlax.</t>
+          <t>Tlaxcala</t>
         </is>
       </c>
     </row>
@@ -24247,7 +24247,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Tlax.</t>
+          <t>Tlaxcala</t>
         </is>
       </c>
     </row>
@@ -24304,7 +24304,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Tlax.</t>
+          <t>Tlaxcala</t>
         </is>
       </c>
     </row>
@@ -24361,7 +24361,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Tlax.</t>
+          <t>Tlaxcala</t>
         </is>
       </c>
     </row>
@@ -24418,7 +24418,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Tlax.</t>
+          <t>Tlaxcala</t>
         </is>
       </c>
     </row>
@@ -24475,7 +24475,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Tlax.</t>
+          <t>Tlaxcala</t>
         </is>
       </c>
     </row>
@@ -24532,7 +24532,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Tlax.</t>
+          <t>Tlaxcala</t>
         </is>
       </c>
     </row>
@@ -24589,7 +24589,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>Tlax.</t>
+          <t>Tlaxcala</t>
         </is>
       </c>
     </row>
@@ -24646,7 +24646,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Tlax.</t>
+          <t>Tlaxcala</t>
         </is>
       </c>
     </row>
@@ -24703,7 +24703,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>Tlax.</t>
+          <t>Tlaxcala</t>
         </is>
       </c>
     </row>
@@ -24760,7 +24760,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>Tlax.</t>
+          <t>Tlaxcala</t>
         </is>
       </c>
     </row>
@@ -24817,7 +24817,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>Tlax.</t>
+          <t>Tlaxcala</t>
         </is>
       </c>
     </row>
@@ -24874,7 +24874,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>Tlax.</t>
+          <t>Tlaxcala</t>
         </is>
       </c>
     </row>
@@ -25037,7 +25037,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Ver.</t>
+          <t>Veracruz</t>
         </is>
       </c>
     </row>
@@ -25094,7 +25094,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Ver.</t>
+          <t>Veracruz</t>
         </is>
       </c>
     </row>
@@ -25151,7 +25151,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Ver.</t>
+          <t>Veracruz</t>
         </is>
       </c>
     </row>
@@ -25208,7 +25208,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Ver.</t>
+          <t>Veracruz</t>
         </is>
       </c>
     </row>
@@ -25265,7 +25265,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Ver.</t>
+          <t>Veracruz</t>
         </is>
       </c>
     </row>
@@ -25322,7 +25322,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Ver.</t>
+          <t>Veracruz</t>
         </is>
       </c>
     </row>
@@ -25379,7 +25379,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Ver.</t>
+          <t>Veracruz</t>
         </is>
       </c>
     </row>
@@ -25436,7 +25436,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Ver.</t>
+          <t>Veracruz</t>
         </is>
       </c>
     </row>
@@ -25493,7 +25493,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Ver.</t>
+          <t>Veracruz</t>
         </is>
       </c>
     </row>
@@ -25550,7 +25550,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Ver.</t>
+          <t>Veracruz</t>
         </is>
       </c>
     </row>
@@ -25607,7 +25607,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>Ver.</t>
+          <t>Veracruz</t>
         </is>
       </c>
     </row>
@@ -25664,7 +25664,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Ver.</t>
+          <t>Veracruz</t>
         </is>
       </c>
     </row>
@@ -25721,7 +25721,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>Ver.</t>
+          <t>Veracruz</t>
         </is>
       </c>
     </row>
@@ -25778,7 +25778,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>Ver.</t>
+          <t>Veracruz</t>
         </is>
       </c>
     </row>
@@ -25835,7 +25835,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>Ver.</t>
+          <t>Veracruz</t>
         </is>
       </c>
     </row>
@@ -25892,7 +25892,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>Ver.</t>
+          <t>Veracruz</t>
         </is>
       </c>
     </row>
@@ -26055,7 +26055,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Yuc.</t>
+          <t>Yucatán</t>
         </is>
       </c>
     </row>
@@ -26112,7 +26112,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Yuc.</t>
+          <t>Yucatán</t>
         </is>
       </c>
     </row>
@@ -26169,7 +26169,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Yuc.</t>
+          <t>Yucatán</t>
         </is>
       </c>
     </row>
@@ -26226,7 +26226,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Yuc.</t>
+          <t>Yucatán</t>
         </is>
       </c>
     </row>
@@ -26283,7 +26283,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Yuc.</t>
+          <t>Yucatán</t>
         </is>
       </c>
     </row>
@@ -26340,7 +26340,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Yuc.</t>
+          <t>Yucatán</t>
         </is>
       </c>
     </row>
@@ -26397,7 +26397,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Yuc.</t>
+          <t>Yucatán</t>
         </is>
       </c>
     </row>
@@ -26454,7 +26454,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Yuc.</t>
+          <t>Yucatán</t>
         </is>
       </c>
     </row>
@@ -26511,7 +26511,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Yuc.</t>
+          <t>Yucatán</t>
         </is>
       </c>
     </row>
@@ -26568,7 +26568,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Yuc.</t>
+          <t>Yucatán</t>
         </is>
       </c>
     </row>
@@ -26625,7 +26625,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>Yuc.</t>
+          <t>Yucatán</t>
         </is>
       </c>
     </row>
@@ -26682,7 +26682,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Yuc.</t>
+          <t>Yucatán</t>
         </is>
       </c>
     </row>
@@ -26739,7 +26739,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>Yuc.</t>
+          <t>Yucatán</t>
         </is>
       </c>
     </row>
@@ -26796,7 +26796,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>Yuc.</t>
+          <t>Yucatán</t>
         </is>
       </c>
     </row>
@@ -26853,7 +26853,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>Yuc.</t>
+          <t>Yucatán</t>
         </is>
       </c>
     </row>
@@ -26910,7 +26910,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>Yuc.</t>
+          <t>Yucatán</t>
         </is>
       </c>
     </row>
@@ -27073,7 +27073,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Zac.</t>
+          <t>Zacatecas</t>
         </is>
       </c>
     </row>
@@ -27130,7 +27130,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Zac.</t>
+          <t>Zacatecas</t>
         </is>
       </c>
     </row>
@@ -27187,7 +27187,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Zac.</t>
+          <t>Zacatecas</t>
         </is>
       </c>
     </row>
@@ -27244,7 +27244,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Zac.</t>
+          <t>Zacatecas</t>
         </is>
       </c>
     </row>
@@ -27301,7 +27301,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Zac.</t>
+          <t>Zacatecas</t>
         </is>
       </c>
     </row>
@@ -27358,7 +27358,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Zac.</t>
+          <t>Zacatecas</t>
         </is>
       </c>
     </row>
@@ -27415,7 +27415,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Zac.</t>
+          <t>Zacatecas</t>
         </is>
       </c>
     </row>
@@ -27472,7 +27472,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Zac.</t>
+          <t>Zacatecas</t>
         </is>
       </c>
     </row>
@@ -27529,7 +27529,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Zac.</t>
+          <t>Zacatecas</t>
         </is>
       </c>
     </row>
@@ -27586,7 +27586,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Zac.</t>
+          <t>Zacatecas</t>
         </is>
       </c>
     </row>
@@ -27643,7 +27643,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>Zac.</t>
+          <t>Zacatecas</t>
         </is>
       </c>
     </row>
@@ -27700,7 +27700,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Zac.</t>
+          <t>Zacatecas</t>
         </is>
       </c>
     </row>
@@ -27757,7 +27757,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>Zac.</t>
+          <t>Zacatecas</t>
         </is>
       </c>
     </row>
@@ -27814,7 +27814,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>Zac.</t>
+          <t>Zacatecas</t>
         </is>
       </c>
     </row>
@@ -27871,7 +27871,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>Zac.</t>
+          <t>Zacatecas</t>
         </is>
       </c>
     </row>
@@ -27928,7 +27928,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>Zac.</t>
+          <t>Zacatecas</t>
         </is>
       </c>
     </row>
@@ -28091,7 +28091,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>BCS</t>
+          <t>Baja California Sur</t>
         </is>
       </c>
     </row>
@@ -28148,7 +28148,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>BCS</t>
+          <t>Baja California Sur</t>
         </is>
       </c>
     </row>
@@ -28205,7 +28205,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>BCS</t>
+          <t>Baja California Sur</t>
         </is>
       </c>
     </row>
@@ -28262,7 +28262,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>BCS</t>
+          <t>Baja California Sur</t>
         </is>
       </c>
     </row>
@@ -28319,7 +28319,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>BCS</t>
+          <t>Baja California Sur</t>
         </is>
       </c>
     </row>
@@ -28376,7 +28376,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>BCS</t>
+          <t>Baja California Sur</t>
         </is>
       </c>
     </row>
@@ -28433,7 +28433,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>BCS</t>
+          <t>Baja California Sur</t>
         </is>
       </c>
     </row>
@@ -28490,7 +28490,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>BCS</t>
+          <t>Baja California Sur</t>
         </is>
       </c>
     </row>
@@ -28547,7 +28547,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>BCS</t>
+          <t>Baja California Sur</t>
         </is>
       </c>
     </row>
@@ -28604,7 +28604,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>BCS</t>
+          <t>Baja California Sur</t>
         </is>
       </c>
     </row>
@@ -28661,7 +28661,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>BCS</t>
+          <t>Baja California Sur</t>
         </is>
       </c>
     </row>
@@ -28718,7 +28718,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>BCS</t>
+          <t>Baja California Sur</t>
         </is>
       </c>
     </row>
@@ -28775,7 +28775,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>BCS</t>
+          <t>Baja California Sur</t>
         </is>
       </c>
     </row>
@@ -28832,7 +28832,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>BCS</t>
+          <t>Baja California Sur</t>
         </is>
       </c>
     </row>
@@ -28889,7 +28889,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>BCS</t>
+          <t>Baja California Sur</t>
         </is>
       </c>
     </row>
@@ -28946,7 +28946,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>BCS</t>
+          <t>Baja California Sur</t>
         </is>
       </c>
     </row>
@@ -29109,7 +29109,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Camp.</t>
+          <t>Campeche</t>
         </is>
       </c>
     </row>
@@ -29166,7 +29166,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Camp.</t>
+          <t>Campeche</t>
         </is>
       </c>
     </row>
@@ -29223,7 +29223,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Camp.</t>
+          <t>Campeche</t>
         </is>
       </c>
     </row>
@@ -29280,7 +29280,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Camp.</t>
+          <t>Campeche</t>
         </is>
       </c>
     </row>
@@ -29337,7 +29337,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Camp.</t>
+          <t>Campeche</t>
         </is>
       </c>
     </row>
@@ -29394,7 +29394,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Camp.</t>
+          <t>Campeche</t>
         </is>
       </c>
     </row>
@@ -29451,7 +29451,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Camp.</t>
+          <t>Campeche</t>
         </is>
       </c>
     </row>
@@ -29508,7 +29508,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Camp.</t>
+          <t>Campeche</t>
         </is>
       </c>
     </row>
@@ -29565,7 +29565,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Camp.</t>
+          <t>Campeche</t>
         </is>
       </c>
     </row>
@@ -29622,7 +29622,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Camp.</t>
+          <t>Campeche</t>
         </is>
       </c>
     </row>
@@ -29679,7 +29679,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>Camp.</t>
+          <t>Campeche</t>
         </is>
       </c>
     </row>
@@ -29736,7 +29736,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Camp.</t>
+          <t>Campeche</t>
         </is>
       </c>
     </row>
@@ -29793,7 +29793,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>Camp.</t>
+          <t>Campeche</t>
         </is>
       </c>
     </row>
@@ -29850,7 +29850,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>Camp.</t>
+          <t>Campeche</t>
         </is>
       </c>
     </row>
@@ -29907,7 +29907,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>Camp.</t>
+          <t>Campeche</t>
         </is>
       </c>
     </row>
@@ -29964,7 +29964,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>Camp.</t>
+          <t>Campeche</t>
         </is>
       </c>
     </row>
@@ -30127,7 +30127,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Coah.</t>
+          <t>Coahuila</t>
         </is>
       </c>
     </row>
@@ -30184,7 +30184,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Coah.</t>
+          <t>Coahuila</t>
         </is>
       </c>
     </row>
@@ -30241,7 +30241,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Coah.</t>
+          <t>Coahuila</t>
         </is>
       </c>
     </row>
@@ -30298,7 +30298,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Coah.</t>
+          <t>Coahuila</t>
         </is>
       </c>
     </row>
@@ -30355,7 +30355,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Coah.</t>
+          <t>Coahuila</t>
         </is>
       </c>
     </row>
@@ -30412,7 +30412,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Coah.</t>
+          <t>Coahuila</t>
         </is>
       </c>
     </row>
@@ -30469,7 +30469,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Coah.</t>
+          <t>Coahuila</t>
         </is>
       </c>
     </row>
@@ -30526,7 +30526,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Coah.</t>
+          <t>Coahuila</t>
         </is>
       </c>
     </row>
@@ -30583,7 +30583,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Coah.</t>
+          <t>Coahuila</t>
         </is>
       </c>
     </row>
@@ -30640,7 +30640,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Coah.</t>
+          <t>Coahuila</t>
         </is>
       </c>
     </row>
@@ -30697,7 +30697,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>Coah.</t>
+          <t>Coahuila</t>
         </is>
       </c>
     </row>
@@ -30754,7 +30754,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Coah.</t>
+          <t>Coahuila</t>
         </is>
       </c>
     </row>
@@ -30811,7 +30811,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>Coah.</t>
+          <t>Coahuila</t>
         </is>
       </c>
     </row>
@@ -30868,7 +30868,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>Coah.</t>
+          <t>Coahuila</t>
         </is>
       </c>
     </row>
@@ -30925,7 +30925,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>Coah.</t>
+          <t>Coahuila</t>
         </is>
       </c>
     </row>
@@ -30982,7 +30982,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>Coah.</t>
+          <t>Coahuila</t>
         </is>
       </c>
     </row>
@@ -31145,7 +31145,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Col.</t>
+          <t>Colima</t>
         </is>
       </c>
     </row>
@@ -31202,7 +31202,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Col.</t>
+          <t>Colima</t>
         </is>
       </c>
     </row>
@@ -31259,7 +31259,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Col.</t>
+          <t>Colima</t>
         </is>
       </c>
     </row>
@@ -31316,7 +31316,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Col.</t>
+          <t>Colima</t>
         </is>
       </c>
     </row>
@@ -31373,7 +31373,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Col.</t>
+          <t>Colima</t>
         </is>
       </c>
     </row>
@@ -31430,7 +31430,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Col.</t>
+          <t>Colima</t>
         </is>
       </c>
     </row>
@@ -31487,7 +31487,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Col.</t>
+          <t>Colima</t>
         </is>
       </c>
     </row>
@@ -31544,7 +31544,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Col.</t>
+          <t>Colima</t>
         </is>
       </c>
     </row>
@@ -31601,7 +31601,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Col.</t>
+          <t>Colima</t>
         </is>
       </c>
     </row>
@@ -31658,7 +31658,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Col.</t>
+          <t>Colima</t>
         </is>
       </c>
     </row>
@@ -31715,7 +31715,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>Col.</t>
+          <t>Colima</t>
         </is>
       </c>
     </row>
@@ -31772,7 +31772,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Col.</t>
+          <t>Colima</t>
         </is>
       </c>
     </row>
@@ -31829,7 +31829,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>Col.</t>
+          <t>Colima</t>
         </is>
       </c>
     </row>
@@ -31886,7 +31886,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>Col.</t>
+          <t>Colima</t>
         </is>
       </c>
     </row>
@@ -31943,7 +31943,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>Col.</t>
+          <t>Colima</t>
         </is>
       </c>
     </row>
@@ -32000,7 +32000,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>Col.</t>
+          <t>Colima</t>
         </is>
       </c>
     </row>
@@ -32163,7 +32163,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Chis.</t>
+          <t>Chiapas</t>
         </is>
       </c>
     </row>
@@ -32220,7 +32220,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Chis.</t>
+          <t>Chiapas</t>
         </is>
       </c>
     </row>
@@ -32277,7 +32277,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Chis.</t>
+          <t>Chiapas</t>
         </is>
       </c>
     </row>
@@ -32334,7 +32334,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Chis.</t>
+          <t>Chiapas</t>
         </is>
       </c>
     </row>
@@ -32391,7 +32391,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Chis.</t>
+          <t>Chiapas</t>
         </is>
       </c>
     </row>
@@ -32448,7 +32448,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Chis.</t>
+          <t>Chiapas</t>
         </is>
       </c>
     </row>
@@ -32505,7 +32505,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Chis.</t>
+          <t>Chiapas</t>
         </is>
       </c>
     </row>
@@ -32562,7 +32562,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Chis.</t>
+          <t>Chiapas</t>
         </is>
       </c>
     </row>
@@ -32619,7 +32619,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Chis.</t>
+          <t>Chiapas</t>
         </is>
       </c>
     </row>
@@ -32676,7 +32676,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Chis.</t>
+          <t>Chiapas</t>
         </is>
       </c>
     </row>
@@ -32733,7 +32733,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>Chis.</t>
+          <t>Chiapas</t>
         </is>
       </c>
     </row>
@@ -32790,7 +32790,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Chis.</t>
+          <t>Chiapas</t>
         </is>
       </c>
     </row>
@@ -32847,7 +32847,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>Chis.</t>
+          <t>Chiapas</t>
         </is>
       </c>
     </row>
@@ -32904,7 +32904,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>Chis.</t>
+          <t>Chiapas</t>
         </is>
       </c>
     </row>
@@ -32961,7 +32961,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>Chis.</t>
+          <t>Chiapas</t>
         </is>
       </c>
     </row>
@@ -33018,7 +33018,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>Chis.</t>
+          <t>Chiapas</t>
         </is>
       </c>
     </row>
@@ -33181,7 +33181,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Chih.</t>
+          <t>Chihuahua</t>
         </is>
       </c>
     </row>
@@ -33238,7 +33238,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Chih.</t>
+          <t>Chihuahua</t>
         </is>
       </c>
     </row>
@@ -33295,7 +33295,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Chih.</t>
+          <t>Chihuahua</t>
         </is>
       </c>
     </row>
@@ -33352,7 +33352,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Chih.</t>
+          <t>Chihuahua</t>
         </is>
       </c>
     </row>
@@ -33409,7 +33409,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Chih.</t>
+          <t>Chihuahua</t>
         </is>
       </c>
     </row>
@@ -33466,7 +33466,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Chih.</t>
+          <t>Chihuahua</t>
         </is>
       </c>
     </row>
@@ -33523,7 +33523,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Chih.</t>
+          <t>Chihuahua</t>
         </is>
       </c>
     </row>
@@ -33580,7 +33580,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Chih.</t>
+          <t>Chihuahua</t>
         </is>
       </c>
     </row>
@@ -33637,7 +33637,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Chih.</t>
+          <t>Chihuahua</t>
         </is>
       </c>
     </row>
@@ -33694,7 +33694,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Chih.</t>
+          <t>Chihuahua</t>
         </is>
       </c>
     </row>
@@ -33751,7 +33751,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>Chih.</t>
+          <t>Chihuahua</t>
         </is>
       </c>
     </row>
@@ -33808,7 +33808,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Chih.</t>
+          <t>Chihuahua</t>
         </is>
       </c>
     </row>
@@ -33865,7 +33865,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>Chih.</t>
+          <t>Chihuahua</t>
         </is>
       </c>
     </row>
@@ -33922,7 +33922,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>Chih.</t>
+          <t>Chihuahua</t>
         </is>
       </c>
     </row>
@@ -33979,7 +33979,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>Chih.</t>
+          <t>Chihuahua</t>
         </is>
       </c>
     </row>
@@ -34036,7 +34036,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>Chih.</t>
+          <t>Chihuahua</t>
         </is>
       </c>
     </row>

</xml_diff>